<commit_message>
Extend data ingestion prototype to work for 5 different tables.
</commit_message>
<xml_diff>
--- a/app/data_ingestion/interventions.xlsx
+++ b/app/data_ingestion/interventions.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\roghan\repo\Excel_Parsing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\roghan\repo\Tech-Titans\app\data_ingestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5AE921-63C8-4954-808D-AF24A6623618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54A51D5-BAE8-4D12-AE30-5677152744CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6C3C5D19-0FED-4BBB-8FDA-7CF898EDE000}"/>
+    <workbookView xWindow="32130" yWindow="3090" windowWidth="22845" windowHeight="11295" activeTab="4" xr2:uid="{6C3C5D19-0FED-4BBB-8FDA-7CF898EDE000}"/>
   </bookViews>
   <sheets>
     <sheet name="interventions" sheetId="1" r:id="rId1"/>
     <sheet name="themes" sheetId="2" r:id="rId2"/>
     <sheet name="metric_effects" sheetId="3" r:id="rId3"/>
     <sheet name="intervention_effects" sheetId="4" r:id="rId4"/>
+    <sheet name="stages" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -53,12 +54,6 @@
     <t>base_effectiveness</t>
   </si>
   <si>
-    <t>dog</t>
-  </si>
-  <si>
-    <t>food</t>
-  </si>
-  <si>
     <t>cause</t>
   </si>
   <si>
@@ -80,10 +75,40 @@
     <t>cause_intervention</t>
   </si>
   <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>chocolate</t>
+    <t>src_intervention_id</t>
+  </si>
+  <si>
+    <t>dst_intervention_id</t>
+  </si>
+  <si>
+    <t>relation_type</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>test theme two</t>
+  </si>
+  <si>
+    <t>test theme one</t>
+  </si>
+  <si>
+    <t>external_wall_area</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>prereq</t>
   </si>
 </sst>
 </file>
@@ -457,13 +482,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1E4E17-1781-4141-988F-DC806A537FAE}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -483,10 +507,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -497,10 +521,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>501</v>
+        <v>601</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -511,10 +535,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>502</v>
+        <v>602</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -525,10 +549,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>503</v>
+        <v>603</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -544,13 +568,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F2C6DC-232B-43C1-B390-D975F92D1869}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -560,6 +587,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>500</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>501</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -567,15 +610,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24CA556-282B-40CC-AD83-F9152C3A904E}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -587,22 +631,45 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>500</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>600</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>999</v>
+      </c>
+      <c r="F2">
+        <v>9999</v>
+      </c>
+      <c r="G2">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
@@ -612,10 +679,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEF59BD-891B-4465-A58F-8216C89F0E31}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,22 +698,87 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>501</v>
+      </c>
+      <c r="B2">
+        <v>601</v>
+      </c>
+      <c r="C2">
+        <v>600</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>0.99</v>
+      </c>
+      <c r="F2">
+        <v>1.99</v>
+      </c>
+      <c r="G2">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA9C15C-C36F-4C8E-8538-8A03A992687E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>600</v>
+      </c>
+      <c r="B2">
+        <v>603</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve data ingestion (user doesn't need to enter IDs, + other niceties), integrate Mkdocs + mkdocstrings
</commit_message>
<xml_diff>
--- a/app/data_ingestion/interventions.xlsx
+++ b/app/data_ingestion/interventions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\roghan\repo\Tech-Titans\app\data_ingestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54A51D5-BAE8-4D12-AE30-5677152744CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE51668-A804-46F9-83D6-6C120BCA6F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32130" yWindow="3090" windowWidth="22845" windowHeight="11295" activeTab="4" xr2:uid="{6C3C5D19-0FED-4BBB-8FDA-7CF898EDE000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6C3C5D19-0FED-4BBB-8FDA-7CF898EDE000}"/>
   </bookViews>
   <sheets>
     <sheet name="interventions" sheetId="1" r:id="rId1"/>
@@ -40,26 +40,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>theme_id</t>
-  </si>
-  <si>
     <t>base_effectiveness</t>
   </si>
   <si>
-    <t>cause</t>
-  </si>
-  <si>
-    <t>effected_intervention</t>
-  </si>
-  <si>
     <t>metric_type</t>
   </si>
   <si>
@@ -72,36 +60,9 @@
     <t>multiplier</t>
   </si>
   <si>
-    <t>cause_intervention</t>
-  </si>
-  <si>
-    <t>src_intervention_id</t>
-  </si>
-  <si>
-    <t>dst_intervention_id</t>
-  </si>
-  <si>
     <t>relation_type</t>
   </si>
   <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>two</t>
-  </si>
-  <si>
-    <t>three</t>
-  </si>
-  <si>
-    <t>four</t>
-  </si>
-  <si>
-    <t>test theme two</t>
-  </si>
-  <si>
-    <t>test theme one</t>
-  </si>
-  <si>
     <t>external_wall_area</t>
   </si>
   <si>
@@ -109,6 +70,60 @@
   </si>
   <si>
     <t>prereq</t>
+  </si>
+  <si>
+    <t>theme_name</t>
+  </si>
+  <si>
+    <t>src_intervention_name</t>
+  </si>
+  <si>
+    <t>dst_intervention_name</t>
+  </si>
+  <si>
+    <t>cause_intervention_name</t>
+  </si>
+  <si>
+    <t>effected_intervention_name</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Walter</t>
+  </si>
+  <si>
+    <t>Kid</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>cause_name</t>
+  </si>
+  <si>
+    <t>is_stage</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>kid</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>Weak Negative</t>
   </si>
 </sst>
 </file>
@@ -483,11 +498,13 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -496,69 +513,69 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>600</v>
+      <c r="A2" t="s">
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
         <v>2.4</v>
       </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>601</v>
+      <c r="A3" t="s">
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
         <v>4</v>
       </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>602</v>
+      <c r="A4" t="s">
+        <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>6.3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>603</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
         <v>9.1999999999999993</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -568,39 +585,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F2C6DC-232B-43C1-B390-D975F92D1869}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>500</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>501</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -610,66 +619,61 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24CA556-282B-40CC-AD83-F9152C3A904E}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>500</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>600</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
+      <c r="D2">
+        <v>999</v>
       </c>
       <c r="E2">
-        <v>999</v>
-      </c>
-      <c r="F2">
         <v>9999</v>
       </c>
-      <c r="G2">
-        <v>1.5</v>
+      <c r="F2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -679,63 +683,58 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEF59BD-891B-4465-A58F-8216C89F0E31}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="6" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>501</v>
-      </c>
-      <c r="B2">
-        <v>601</v>
-      </c>
-      <c r="C2">
-        <v>600</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
+      <c r="D2">
+        <v>0.99</v>
       </c>
       <c r="E2">
-        <v>0.99</v>
+        <v>1.99</v>
       </c>
       <c r="F2">
-        <v>1.99</v>
-      </c>
-      <c r="G2">
         <v>1.5</v>
       </c>
     </row>
@@ -748,14 +747,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA9C15C-C36F-4C8E-8538-8A03A992687E}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -767,18 +766,18 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>600</v>
-      </c>
-      <c r="B2">
-        <v>603</v>
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>